<commit_message>
Reading file from JSON + Extent Report for passed test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -31,46 +31,25 @@
     <t xml:space="preserve">firstname</t>
   </si>
   <si>
-    <t xml:space="preserve">deepender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abcd</t>
+    <t xml:space="preserve">Admin</t>
+  </si>
+  <si>
+    <t xml:space="preserve">admin123</t>
   </si>
   <si>
     <t xml:space="preserve">Deepender</t>
   </si>
   <si>
-    <t xml:space="preserve">shailu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">abffff</t>
-  </si>
-  <si>
     <t xml:space="preserve">Kanwar</t>
   </si>
   <si>
-    <t xml:space="preserve">indu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dfklsjdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">Indu</t>
   </si>
   <si>
-    <t xml:space="preserve">narender</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fdsjfslkjdf</t>
-  </si>
-  <si>
     <t xml:space="preserve">Narender</t>
   </si>
   <si>
     <t xml:space="preserve">datar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fjslkdfjsll</t>
   </si>
   <si>
     <t xml:space="preserve">Datar</t>
@@ -83,7 +62,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -104,6 +83,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -148,12 +132,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -177,10 +165,10 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -206,46 +194,46 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="1" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="0" t="s">
-        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Adding extent report + Method interceptor + screenshot
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/testData.xlsx
+++ b/src/test/resources/excel/testData.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
   <si>
     <t xml:space="preserve">username</t>
   </si>
@@ -40,15 +40,6 @@
     <t xml:space="preserve">Deepender</t>
   </si>
   <si>
-    <t xml:space="preserve">Kanwar</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Indu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Narender</t>
-  </si>
-  <si>
     <t xml:space="preserve">datar</t>
   </si>
   <si>
@@ -62,7 +53,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -83,11 +74,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -132,16 +118,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -162,13 +144,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -194,46 +176,13 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="1" t="s">
         <v>4</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" s="1" t="s">
         <v>7</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>